<commit_message>
Alteracoes na rota de gerar a planilha do excel e no frontend para deixa-lo mais bonito
</commit_message>
<xml_diff>
--- a/backend/src/assets/teste.xlsx
+++ b/backend/src/assets/teste.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>E-mail:</t>
   </si>
@@ -175,33 +175,9 @@
     <t>SIM-9090-1</t>
   </si>
   <si>
-    <t>SIM-9090-2</t>
-  </si>
-  <si>
-    <t>SIM-9090-3</t>
-  </si>
-  <si>
-    <t>SIM-9090-4</t>
-  </si>
-  <si>
-    <t>SIM-9090-5</t>
-  </si>
-  <si>
     <t>NÃO-9090-1</t>
   </si>
   <si>
-    <t>NÃO-9090-2</t>
-  </si>
-  <si>
-    <t>NÃO-9090-3</t>
-  </si>
-  <si>
-    <t>NÃO-9090-4</t>
-  </si>
-  <si>
-    <t>NÃO-9090-5</t>
-  </si>
-  <si>
     <t>PATIO DE POUSO</t>
   </si>
   <si>
@@ -209,18 +185,6 @@
   </si>
   <si>
     <t>BOCA DE LOBO 1</t>
-  </si>
-  <si>
-    <t>BOCA DE LOBO 2</t>
-  </si>
-  <si>
-    <t>BOCA DE LOBO 3</t>
-  </si>
-  <si>
-    <t>BOCA DE LOBO 4</t>
-  </si>
-  <si>
-    <t>BOCA DE LOBO 5</t>
   </si>
   <si>
     <t>GRD - GUIA DE REMESSA DE DEINONICHUS (DINOSSAURO)</t>
@@ -423,7 +387,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -455,19 +419,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -482,7 +433,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
@@ -640,9 +591,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
@@ -703,15 +651,9 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -740,9 +682,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -751,6 +690,27 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -797,7 +757,7 @@
         <xdr:cNvPr id="3" name="Imagem 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1D8E3282-C8CD-4ECC-9A38-0072B08FE5B8}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D8E3282-C8CD-4ECC-9A38-0072B08FE5B8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1122,8 +1082,8 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:Q990"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1138,26 +1098,26 @@
     <col min="10" max="10" width="8.5703125" style="36" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" style="35" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="25.7109375" style="35" customWidth="1"/>
-    <col min="13" max="13" width="15" style="45" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="45" customWidth="1"/>
-    <col min="15" max="16" width="9.140625" style="45"/>
-    <col min="17" max="17" width="9.140625" style="59"/>
+    <col min="13" max="13" width="15" style="44" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="44" customWidth="1"/>
+    <col min="15" max="16" width="9.140625" style="44"/>
+    <col min="17" max="17" width="9.140625" style="58"/>
     <col min="18" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="55.5" customHeight="1" thickBot="1">
-      <c r="B1" s="46"/>
-      <c r="C1" s="60"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="59"/>
       <c r="D1" s="1"/>
       <c r="E1" s="26"/>
       <c r="F1" s="26"/>
       <c r="G1" s="26"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="67"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="64"/>
     </row>
     <row r="2" spans="1:16" ht="15">
       <c r="A2" s="2"/>
@@ -1172,28 +1132,28 @@
       <c r="J2" s="8"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
     </row>
     <row r="3" spans="1:16" ht="18.75" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
-      <c r="C3" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
+      <c r="C3" s="69" t="s">
+        <v>56</v>
+      </c>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
       <c r="I3" s="29"/>
       <c r="J3" s="29"/>
       <c r="K3" s="33"/>
       <c r="L3" s="33"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
+      <c r="O3" s="41"/>
     </row>
     <row r="4" spans="1:16" ht="10.5" customHeight="1">
       <c r="A4" s="2"/>
@@ -1208,11 +1168,11 @@
       <c r="J4" s="29"/>
       <c r="K4" s="33"/>
       <c r="L4" s="33"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-    </row>
-    <row r="5" spans="1:16" s="50" customFormat="1" ht="16.5">
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+    </row>
+    <row r="5" spans="1:16" s="49" customFormat="1" ht="16.5">
       <c r="A5" s="18"/>
       <c r="B5" s="6"/>
       <c r="C5" s="19"/>
@@ -1227,10 +1187,10 @@
       <c r="J5" s="12"/>
       <c r="K5" s="30"/>
       <c r="L5" s="30"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="43"/>
-      <c r="O5" s="43"/>
-      <c r="P5" s="68"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="65"/>
     </row>
     <row r="6" spans="1:16" ht="16.5">
       <c r="A6" s="2"/>
@@ -1247,9 +1207,9 @@
       <c r="J6" s="8"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
     </row>
     <row r="7" spans="1:16" ht="16.5">
       <c r="A7" s="2"/>
@@ -1266,9 +1226,9 @@
       <c r="J7" s="8"/>
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
-      <c r="M7" s="42"/>
-      <c r="N7" s="42"/>
-      <c r="O7" s="42"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="41"/>
     </row>
     <row r="8" spans="1:16" ht="5.25" customHeight="1">
       <c r="A8" s="2"/>
@@ -1283,11 +1243,11 @@
       <c r="J8" s="8"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="42"/>
-      <c r="N8" s="42"/>
-      <c r="O8" s="42"/>
-    </row>
-    <row r="9" spans="1:16" s="51" customFormat="1" ht="15.75">
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="41"/>
+    </row>
+    <row r="9" spans="1:16" s="50" customFormat="1" ht="15.75">
       <c r="A9" s="13"/>
       <c r="B9" s="14"/>
       <c r="C9" s="15"/>
@@ -1302,10 +1262,10 @@
       <c r="J9" s="16"/>
       <c r="K9" s="27"/>
       <c r="L9" s="27"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="57"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="56"/>
     </row>
     <row r="10" spans="1:16" ht="10.5" customHeight="1">
       <c r="A10" s="2"/>
@@ -1320,9 +1280,9 @@
       <c r="J10" s="8"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="42"/>
-      <c r="O10" s="42"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="41"/>
     </row>
     <row r="11" spans="1:16" ht="15.75">
       <c r="A11" s="2"/>
@@ -1341,9 +1301,9 @@
       <c r="J11" s="8"/>
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="42"/>
-      <c r="O11" s="42"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="41"/>
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1">
       <c r="A12" s="2"/>
@@ -1362,9 +1322,9 @@
       <c r="J12" s="28"/>
       <c r="K12" s="31"/>
       <c r="L12" s="31"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="42"/>
-      <c r="O12" s="42"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="41"/>
     </row>
     <row r="13" spans="1:16" ht="15" customHeight="1">
       <c r="A13" s="2"/>
@@ -1383,9 +1343,9 @@
       <c r="J13" s="28"/>
       <c r="K13" s="31"/>
       <c r="L13" s="31"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="42"/>
-      <c r="O13" s="42"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="41"/>
     </row>
     <row r="14" spans="1:16" ht="15" customHeight="1">
       <c r="A14" s="2"/>
@@ -1404,9 +1364,9 @@
       <c r="J14" s="28"/>
       <c r="K14" s="31"/>
       <c r="L14" s="31"/>
-      <c r="M14" s="42"/>
-      <c r="N14" s="42"/>
-      <c r="O14" s="42"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="41"/>
     </row>
     <row r="15" spans="1:16" ht="15" customHeight="1">
       <c r="A15" s="2"/>
@@ -1414,7 +1374,7 @@
       <c r="C15" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="68" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="23"/>
@@ -1425,9 +1385,9 @@
       <c r="J15" s="28"/>
       <c r="K15" s="31"/>
       <c r="L15" s="31"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
     </row>
     <row r="16" spans="1:16" ht="15" customHeight="1">
       <c r="A16" s="2"/>
@@ -1446,9 +1406,9 @@
       <c r="J16" s="20"/>
       <c r="K16" s="32"/>
       <c r="L16" s="32"/>
-      <c r="M16" s="42"/>
-      <c r="N16" s="42"/>
-      <c r="O16" s="42"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="41"/>
     </row>
     <row r="17" spans="1:15" ht="10.5" customHeight="1">
       <c r="A17" s="2"/>
@@ -1463,9 +1423,9 @@
       <c r="J17" s="29"/>
       <c r="K17" s="33"/>
       <c r="L17" s="33"/>
-      <c r="M17" s="42"/>
-      <c r="N17" s="42"/>
-      <c r="O17" s="42"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="41"/>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="2"/>
@@ -1480,9 +1440,9 @@
       <c r="J18" s="29"/>
       <c r="K18" s="33"/>
       <c r="L18" s="33"/>
-      <c r="M18" s="42"/>
-      <c r="N18" s="42"/>
-      <c r="O18" s="42"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1">
       <c r="A19" s="2"/>
@@ -1490,7 +1450,7 @@
       <c r="C19" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="70" t="s">
+      <c r="D19" s="67" t="s">
         <v>49</v>
       </c>
       <c r="E19" s="8"/>
@@ -1501,9 +1461,9 @@
       <c r="J19" s="29"/>
       <c r="K19" s="33"/>
       <c r="L19" s="33"/>
-      <c r="M19" s="42"/>
-      <c r="N19" s="42"/>
-      <c r="O19" s="42"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="41"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1">
       <c r="A20" s="2"/>
@@ -1522,8 +1482,8 @@
       <c r="J20" s="24"/>
       <c r="K20" s="22"/>
       <c r="L20" s="22"/>
-      <c r="M20" s="42"/>
-      <c r="N20" s="42"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1">
       <c r="A21" s="2"/>
@@ -1542,9 +1502,9 @@
       <c r="J21" s="29"/>
       <c r="K21" s="33"/>
       <c r="L21" s="33"/>
-      <c r="M21" s="42"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="41"/>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1">
       <c r="A22" s="2"/>
@@ -1563,9 +1523,9 @@
       <c r="J22" s="29"/>
       <c r="K22" s="33"/>
       <c r="L22" s="33"/>
-      <c r="M22" s="42"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="41"/>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" s="2"/>
@@ -1580,144 +1540,144 @@
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
       <c r="L23" s="5"/>
-      <c r="M23" s="69"/>
-      <c r="N23" s="42"/>
-      <c r="O23" s="42"/>
+      <c r="M23" s="66"/>
+      <c r="N23" s="41"/>
+      <c r="O23" s="41"/>
     </row>
     <row r="24" spans="1:15" ht="21" customHeight="1">
       <c r="A24" s="2"/>
-      <c r="C24" s="58" t="s">
+      <c r="C24" s="57" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="75" t="s">
+      <c r="D24" s="71" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75"/>
-      <c r="H24" s="75"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
       <c r="I24" s="8"/>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
       <c r="L24" s="5"/>
-      <c r="M24" s="69"/>
-      <c r="N24" s="42"/>
-      <c r="O24" s="42"/>
+      <c r="M24" s="66"/>
+      <c r="N24" s="41"/>
+      <c r="O24" s="41"/>
     </row>
     <row r="25" spans="1:15">
-      <c r="B25" s="53"/>
+      <c r="B25" s="52"/>
       <c r="C25" s="36"/>
       <c r="J25" s="28"/>
       <c r="K25" s="28"/>
       <c r="L25" s="31"/>
-      <c r="M25" s="69"/>
+      <c r="M25" s="66"/>
     </row>
     <row r="26" spans="1:15">
-      <c r="B26" s="53"/>
-      <c r="C26" s="52" t="s">
+      <c r="B26" s="52"/>
+      <c r="C26" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="74" t="s">
+      <c r="F26" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="74"/>
-      <c r="I26" s="54"/>
+      <c r="G26" s="70"/>
+      <c r="I26" s="53"/>
       <c r="J26" s="28"/>
       <c r="K26" s="28"/>
       <c r="L26" s="31"/>
-      <c r="M26" s="69"/>
+      <c r="M26" s="66"/>
     </row>
     <row r="27" spans="1:15">
-      <c r="B27" s="53"/>
-      <c r="C27" s="64" t="s">
+      <c r="B27" s="52"/>
+      <c r="C27" s="61" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="64"/>
-      <c r="E27" s="64"/>
-      <c r="F27" s="64" t="s">
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="G27" s="66"/>
-      <c r="I27" s="55"/>
+      <c r="G27" s="63"/>
+      <c r="I27" s="54"/>
       <c r="J27" s="28"/>
       <c r="K27" s="28"/>
       <c r="L27" s="31"/>
-      <c r="M27" s="69"/>
+      <c r="M27" s="66"/>
     </row>
     <row r="28" spans="1:15">
-      <c r="B28" s="53"/>
-      <c r="C28" s="50" t="s">
+      <c r="B28" s="52"/>
+      <c r="C28" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="64"/>
-      <c r="E28" s="64"/>
-      <c r="F28" s="64" t="s">
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="G28" s="66"/>
-      <c r="I28" s="55"/>
+      <c r="G28" s="63"/>
+      <c r="I28" s="54"/>
       <c r="J28" s="28"/>
       <c r="K28" s="28"/>
       <c r="L28" s="31"/>
-      <c r="M28" s="69"/>
+      <c r="M28" s="66"/>
     </row>
     <row r="29" spans="1:15">
-      <c r="B29" s="53"/>
-      <c r="C29" s="50" t="s">
+      <c r="B29" s="52"/>
+      <c r="C29" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="64"/>
-      <c r="E29" s="64"/>
-      <c r="F29" s="64" t="s">
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="66"/>
-      <c r="I29" s="55"/>
+      <c r="G29" s="63"/>
+      <c r="I29" s="54"/>
       <c r="J29" s="28"/>
       <c r="K29" s="28"/>
       <c r="L29" s="31"/>
-      <c r="M29" s="69"/>
+      <c r="M29" s="66"/>
     </row>
     <row r="30" spans="1:15">
-      <c r="B30" s="53"/>
-      <c r="C30" s="50" t="s">
+      <c r="B30" s="52"/>
+      <c r="C30" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="64"/>
-      <c r="E30" s="64"/>
-      <c r="F30" s="65"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="55"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="54"/>
       <c r="J30" s="28"/>
       <c r="K30" s="28"/>
       <c r="L30" s="31"/>
-      <c r="M30" s="69"/>
+      <c r="M30" s="66"/>
     </row>
     <row r="31" spans="1:15">
-      <c r="B31" s="53"/>
-      <c r="C31" s="50" t="s">
+      <c r="B31" s="52"/>
+      <c r="C31" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="65"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="55"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="63"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="54"/>
       <c r="J31" s="28"/>
       <c r="K31" s="28"/>
       <c r="L31" s="31"/>
-      <c r="M31" s="69"/>
+      <c r="M31" s="66"/>
     </row>
     <row r="32" spans="1:15" ht="6" customHeight="1">
-      <c r="C32" s="50"/>
-      <c r="D32" s="50"/>
-      <c r="E32" s="66"/>
-      <c r="F32" s="66"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="66"/>
-      <c r="O32" s="56">
+      <c r="C32" s="49"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
+      <c r="O32" s="55">
         <v>1</v>
       </c>
     </row>
@@ -1756,191 +1716,111 @@
       <c r="L33" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="N33" s="57" t="s">
+      <c r="N33" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="O33" s="56">
+      <c r="O33" s="55">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="18">
-      <c r="B34" s="62">
+      <c r="B34" s="60">
         <v>1</v>
       </c>
-      <c r="C34" s="63" t="s">
+      <c r="C34" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="E34" s="63">
+      <c r="D34" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="E34" s="60">
         <v>0</v>
       </c>
-      <c r="F34" s="63" t="s">
+      <c r="F34" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="G34" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="H34" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="I34" s="72" t="s">
-        <v>63</v>
-      </c>
-      <c r="J34" s="41">
+      <c r="G34" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="H34" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="I34" s="76" t="s">
+        <v>55</v>
+      </c>
+      <c r="J34" s="77">
         <v>1</v>
       </c>
-      <c r="K34" s="41" t="s">
+      <c r="K34" s="77" t="s">
         <v>20</v>
       </c>
-      <c r="L34" s="61"/>
-      <c r="N34" s="57"/>
-      <c r="O34" s="56"/>
+      <c r="L34" s="78"/>
+      <c r="N34" s="56"/>
+      <c r="O34" s="55"/>
     </row>
     <row r="35" spans="1:15" ht="18">
-      <c r="B35" s="62">
-        <v>2</v>
-      </c>
-      <c r="C35" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="E35" s="63">
-        <v>0</v>
-      </c>
-      <c r="F35" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="H35" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="I35" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="J35" s="41">
-        <v>1</v>
-      </c>
-      <c r="K35" s="41" t="s">
+      <c r="B35" s="72"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="72"/>
+      <c r="E35" s="72"/>
+      <c r="F35" s="72"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="73"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="75"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="55"/>
+    </row>
+    <row r="36" spans="1:15" ht="18">
+      <c r="B36" s="72"/>
+      <c r="C36" s="72"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="72"/>
+      <c r="F36" s="72"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="73"/>
+      <c r="I36" s="73"/>
+      <c r="J36" s="74"/>
+      <c r="K36" s="74"/>
+      <c r="L36" s="75"/>
+      <c r="N36" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="L35" s="61"/>
-      <c r="N35" s="57"/>
-      <c r="O35" s="56"/>
-    </row>
-    <row r="36" spans="1:15" ht="18">
-      <c r="B36" s="62">
-        <v>3</v>
-      </c>
-      <c r="C36" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="D36" s="63" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36" s="63">
-        <v>0</v>
-      </c>
-      <c r="F36" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="H36" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="I36" s="72" t="s">
-        <v>65</v>
-      </c>
-      <c r="J36" s="41">
-        <v>1</v>
-      </c>
-      <c r="K36" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="L36" s="61"/>
-      <c r="N36" s="57" t="s">
-        <v>20</v>
-      </c>
-      <c r="O36" s="56">
+      <c r="O36" s="55">
         <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="18">
-      <c r="B37" s="62">
-        <v>4</v>
-      </c>
-      <c r="C37" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="D37" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="E37" s="63">
-        <v>0</v>
-      </c>
-      <c r="F37" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="H37" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="I37" s="72" t="s">
-        <v>66</v>
-      </c>
-      <c r="J37" s="41">
-        <v>1</v>
-      </c>
-      <c r="K37" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="L37" s="61"/>
-      <c r="N37" s="57"/>
-      <c r="O37" s="56"/>
+      <c r="B37" s="72"/>
+      <c r="C37" s="72"/>
+      <c r="D37" s="72"/>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="73"/>
+      <c r="J37" s="74"/>
+      <c r="K37" s="74"/>
+      <c r="L37" s="75"/>
+      <c r="N37" s="56"/>
+      <c r="O37" s="55"/>
     </row>
     <row r="38" spans="1:15" ht="18">
-      <c r="B38" s="62">
-        <v>5</v>
-      </c>
-      <c r="C38" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="D38" s="63" t="s">
-        <v>60</v>
-      </c>
-      <c r="E38" s="63">
-        <v>0</v>
-      </c>
-      <c r="F38" s="63" t="s">
-        <v>38</v>
-      </c>
-      <c r="G38" s="72" t="s">
-        <v>61</v>
-      </c>
-      <c r="H38" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="I38" s="72" t="s">
-        <v>67</v>
-      </c>
-      <c r="J38" s="41">
-        <v>1</v>
-      </c>
-      <c r="K38" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="L38" s="61"/>
-      <c r="N38" s="57"/>
-      <c r="O38" s="56"/>
+      <c r="B38" s="72"/>
+      <c r="C38" s="72"/>
+      <c r="D38" s="72"/>
+      <c r="E38" s="72"/>
+      <c r="F38" s="72"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="73"/>
+      <c r="J38" s="74"/>
+      <c r="K38" s="74"/>
+      <c r="L38" s="75"/>
+      <c r="N38" s="56"/>
+      <c r="O38" s="55"/>
     </row>
     <row r="39" spans="1:15" ht="20.100000000000001" customHeight="1"/>
     <row r="40" spans="1:15" ht="20.100000000000001" customHeight="1"/>
@@ -1955,7 +1835,7 @@
     <row r="42" spans="1:15" ht="20.100000000000001" customHeight="1"/>
     <row r="43" spans="1:15" ht="20.100000000000001" customHeight="1"/>
     <row r="44" spans="1:15" ht="20.100000000000001" customHeight="1">
-      <c r="C44" s="59" t="s">
+      <c r="C44" s="58" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Commitando a funcionalidade de baixar o arquivo xlsx no backend e no frontend
</commit_message>
<xml_diff>
--- a/backend/src/assets/teste.xlsx
+++ b/backend/src/assets/teste.xlsx
@@ -1082,8 +1082,8 @@
   <sheetPr codeName="Plan1"/>
   <dimension ref="A1:Q990"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>